<commit_message>
Processed net load results for D25M25 D50M0 and W120S1A 600 GW scenarios - again all files
</commit_message>
<xml_diff>
--- a/india_REV_input/Scenarios_Cost_Master_v4.xlsx
+++ b/india_REV_input/Scenarios_Cost_Master_v4.xlsx
@@ -2401,10 +2401,10 @@
   <dimension ref="A1:AC45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="U9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="U21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="Z7" sqref="Z7"/>
+      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Processed screening curves for all scenarios
</commit_message>
<xml_diff>
--- a/india_REV_input/Scenarios_Cost_Master_v4.xlsx
+++ b/india_REV_input/Scenarios_Cost_Master_v4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30495" yWindow="-3600" windowWidth="25035" windowHeight="14955"/>
+    <workbookView xWindow="-30495" yWindow="-3600" windowWidth="25035" windowHeight="14955" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="REvalue_input_csv" sheetId="11" r:id="rId1"/>
@@ -1122,18 +1122,9 @@
     <t>scenario_coal_gas</t>
   </si>
   <si>
-    <t>scenario_wind (blank for base)</t>
-  </si>
-  <si>
-    <t>scenario_solar (blank for base)</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
-    <t>scenario_battery (blank for base)</t>
-  </si>
-  <si>
     <t>Battery Capital Cost (USD/kW)</t>
   </si>
   <si>
@@ -1900,6 +1891,15 @@
   </si>
   <si>
     <t>percentage, 50p is base</t>
+  </si>
+  <si>
+    <t>scenario_wind</t>
+  </si>
+  <si>
+    <t>scenario_solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario_battery </t>
   </si>
 </sst>
 </file>
@@ -2412,11 +2412,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,102 +2445,102 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G1" t="s">
         <v>228</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>229</v>
       </c>
-      <c r="C1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>230</v>
       </c>
-      <c r="E1" t="s">
-        <v>415</v>
-      </c>
-      <c r="F1" t="s">
-        <v>476</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>231</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>232</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>233</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>234</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>235</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>236</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>237</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>238</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>239</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>240</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>241</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>242</v>
       </c>
-      <c r="S1" t="s">
-        <v>243</v>
-      </c>
-      <c r="T1" t="s">
-        <v>244</v>
-      </c>
-      <c r="U1" t="s">
-        <v>245</v>
-      </c>
       <c r="V1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="W1" t="s">
+        <v>419</v>
+      </c>
+      <c r="X1" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>421</v>
+      </c>
+      <c r="Z1" t="s">
         <v>422</v>
       </c>
-      <c r="X1" t="s">
-        <v>423</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>424</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>425</v>
-      </c>
       <c r="AA1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="AB1" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>466</v>
+      </c>
+      <c r="AD1" t="s">
         <v>467</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C2" s="21" t="str">
         <f>C3</f>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE(C10,C13,C17,C19,C21,C25,C29,C33,C36,C39,C42,C44,C47)</f>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:E4" si="4">CONCATENATE(C10,C13,C15,C17,C19,C21,C36,C39,C42,C44,C47)</f>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ref="C5:U5" si="6">CONCATENATE(C11,C17,C19,C21,C36,C39,C42,C44,C47)</f>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:U6" si="9">CONCATENATE(C11,C17,C19,C21,C36,C39,C42,C44,C47)</f>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" ref="C7:U7" si="11">CONCATENATE(C37,"_",C40)</f>
@@ -3242,7 +3242,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C8" t="str">
         <f>CONCATENATE(C11,C29,C33,C25)</f>
@@ -3359,99 +3359,99 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>256</v>
-      </c>
       <c r="E9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="T9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="U9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="W9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="X9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Y9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Z9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AA9" s="21" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="AB9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AC9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AD9" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C10" t="str">
         <f>CONCATENATE("C", LEFT(C9,1), "c")</f>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:U11" si="20">CONCATENATE("coal",LEFT(C9,1), "c")</f>
@@ -3685,10 +3685,10 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C12" s="21">
         <v>70</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C13" t="str">
         <f>CONCATENATE("C",C12,"m")</f>
@@ -3894,10 +3894,10 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C14" s="21">
         <v>50</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C15" t="str">
         <f>IF(C14=50,"",CONCATENATE("G",C14, "m"))</f>
@@ -4103,10 +4103,10 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C16" s="21">
         <v>0</v>
@@ -4195,7 +4195,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ref="C15:U17" si="27">IF(C16=0,"",CONCATENATE("H",C16))</f>
@@ -4312,10 +4312,10 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C18" s="21">
         <v>0</v>
@@ -4404,7 +4404,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ref="C19:U19" si="30">IF(C18=0,"",CONCATENATE("N",C18))</f>
@@ -4521,10 +4521,10 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C20" s="21">
         <v>0</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" ref="C21:U21" si="33">IF(C20=0,"",CONCATENATE("B",C20))</f>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" ref="C22:U22" si="36">CONCATENATE("bat", C20)</f>
@@ -4847,10 +4847,10 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C23" s="21">
         <v>0</v>
@@ -4939,99 +4939,99 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B24" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="N24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="P24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="T24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="U24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="V24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="W24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="X24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Y24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Z24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AA24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AB24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AC24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AD24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C25" t="str">
         <f>IF(C23=0,"",CONCATENATE("B",C23,LEFT(C24,1),"c"))</f>
@@ -5148,7 +5148,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C26" t="str">
         <f>CONCATENATE("battery",UPPER(LEFT(C24,1)), "C",C23)</f>
@@ -5265,10 +5265,10 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C27" s="21">
         <v>0</v>
@@ -5357,99 +5357,99 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B28" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="N28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="P28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="T28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="U28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="V28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="W28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="X28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Y28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Z28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AA28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AB28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AC28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AD28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" ref="C29:U29" si="45">IF(C27=0,"",CONCATENATE("W",C27,LEFT(C28,1),"c"))</f>
@@ -5566,7 +5566,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" ref="C30:U30" si="48">CONCATENATE("wind",UPPER(LEFT(C28,1)), "C",C27)</f>
@@ -5683,10 +5683,10 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C31" s="21">
         <v>0</v>
@@ -5775,99 +5775,99 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B32" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="N32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="P32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Q32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="R32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="T32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="U32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="V32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="W32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="X32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Y32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Z32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AA32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AB32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AC32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AD32" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" ref="C33:N33" si="51">IF(C31=0,"",CONCATENATE("W",C31,LEFT(C32,1),"c"))</f>
@@ -5984,7 +5984,7 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" ref="C34:U34" si="55">CONCATENATE("solar",UPPER(LEFT(C32,1)), "C",C31)</f>
@@ -6101,10 +6101,10 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C35" s="21">
         <v>80</v>
@@ -6193,7 +6193,7 @@
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" ref="C36:U36" si="58">IF(C35=80,"", CONCATENATE("W",C35))</f>
@@ -6310,7 +6310,7 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" ref="C37:U37" si="61">CONCATENATE("W",C35)</f>
@@ -6427,99 +6427,99 @@
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="K38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="L38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="M38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="N38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="O38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="P38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="R38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="S38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="T38" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="U38" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="C38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="J38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="K38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="L38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="M38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="N38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="O38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="P38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="Q38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="R38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="S38" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="T38" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="U38" s="21" t="s">
-        <v>290</v>
-      </c>
       <c r="V38" s="21" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="W38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="X38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Y38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Z38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AA38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AB38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AC38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AD38" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" ref="C39:U39" si="64">IF(C38="0d", "", CONCATENATE("S",C38))</f>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" ref="C40:U40" si="67">CONCATENATE("S",C38)</f>
@@ -6753,7 +6753,7 @@
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="21">
@@ -6843,7 +6843,7 @@
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" ref="C42:U42" si="70">IF(C41=2014,"",CONCATENATE("L",C41))</f>
@@ -6960,99 +6960,99 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="L43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="N43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="O43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="Q43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="R43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="S43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="T43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="U43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="V43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="W43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="X43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="Y43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="Z43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AA43" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AB43" s="21" t="s">
+        <v>465</v>
+      </c>
+      <c r="AC43" s="21" t="s">
         <v>468</v>
       </c>
-      <c r="AC43" s="21" t="s">
-        <v>471</v>
-      </c>
       <c r="AD43" s="21" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" ref="C44:U44" si="73">IF(C43="none","",CONCATENATE("L",C43))</f>
@@ -7169,99 +7169,99 @@
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="M45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="N45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="O45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="Q45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="R45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="S45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="T45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="U45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="V45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="W45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="X45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="Y45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="Z45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="AA45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="AB45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="AC45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="AD45" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -7350,7 +7350,7 @@
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" ref="C47:U47" si="76">IF(C45="RT","",CONCATENATE(C45,C46))</f>
@@ -7493,41 +7493,41 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D3">
         <v>216</v>
@@ -7546,13 +7546,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D4">
         <v>88</v>
@@ -7571,10 +7571,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E5">
         <f>D5/60</f>
@@ -7590,13 +7590,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D6">
         <v>89</v>
@@ -7658,517 +7658,517 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G1" t="s">
         <v>230</v>
       </c>
-      <c r="D1" t="s">
-        <v>415</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>231</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>232</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>233</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>234</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>235</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>236</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>237</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>238</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>239</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>240</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>241</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>242</v>
       </c>
-      <c r="Q1" t="s">
-        <v>243</v>
-      </c>
-      <c r="R1" t="s">
-        <v>244</v>
-      </c>
-      <c r="S1" t="s">
-        <v>245</v>
-      </c>
       <c r="T1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="U1" t="s">
+        <v>419</v>
+      </c>
+      <c r="V1" t="s">
+        <v>420</v>
+      </c>
+      <c r="W1" t="s">
+        <v>421</v>
+      </c>
+      <c r="X1" t="s">
         <v>422</v>
       </c>
-      <c r="V1" t="s">
-        <v>423</v>
-      </c>
-      <c r="W1" t="s">
-        <v>424</v>
-      </c>
-      <c r="X1" t="s">
-        <v>425</v>
-      </c>
       <c r="Y1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="Z1" t="s">
+        <v>464</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>466</v>
+      </c>
+      <c r="AB1" t="s">
         <v>467</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E2" t="s">
         <v>442</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>443</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>444</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>445</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>446</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>447</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>448</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>449</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>450</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>451</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>452</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>453</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>454</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>455</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>456</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>457</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>458</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>459</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>460</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>461</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>462</v>
       </c>
-      <c r="W2" t="s">
-        <v>463</v>
-      </c>
-      <c r="X2" t="s">
-        <v>464</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>465</v>
-      </c>
       <c r="Z2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="AA2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="AB2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="M3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="O3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="P3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="R3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="S3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="T3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="U3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="V3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="W3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="X3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Y3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Z3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="AA3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="AB3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="M4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="O4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="P4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="R4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="S4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="T4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="U4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="V4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="W4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="X4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Y4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Z4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="AA4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="AB4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="M5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="O5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="P5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="R5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="T5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="V5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="X5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Y5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C6" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="M6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="O6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="P6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="R6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="T6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="V6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="X6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Y6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>408</v>
+      </c>
+      <c r="B7" t="s">
         <v>411</v>
       </c>
-      <c r="B7" t="s">
-        <v>414</v>
-      </c>
       <c r="C7" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="J7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="M7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="O7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="P7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Q7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="R7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="T7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="V7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="X7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="Y7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -8186,8 +8186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL73"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="U39" sqref="U39"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9:AE64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8230,7 +8230,7 @@
         <v>65</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
@@ -8282,10 +8282,10 @@
         <v>217</v>
       </c>
       <c r="AK3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AL3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -8341,7 +8341,7 @@
         <v>3.6923076923076925</v>
       </c>
       <c r="AD4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AE4">
         <f>B68</f>
@@ -8352,7 +8352,7 @@
         <v>15</v>
       </c>
       <c r="AG4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AH4">
         <f>C68</f>
@@ -8363,7 +8363,7 @@
         <v>10</v>
       </c>
       <c r="AJ4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AK4">
         <v>2800</v>
@@ -8436,7 +8436,7 @@
         <v>10</v>
       </c>
       <c r="AJ5" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="AK5">
         <f>$AK$4*0.75</f>
@@ -8486,7 +8486,7 @@
         <v>10</v>
       </c>
       <c r="AJ6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="AK6">
         <f>$AK$4*0.5</f>
@@ -8535,7 +8535,7 @@
         <v>3900</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -8655,13 +8655,13 @@
         <v>42.6768</v>
       </c>
       <c r="R11" t="s">
+        <v>477</v>
+      </c>
+      <c r="S11" t="s">
         <v>220</v>
       </c>
-      <c r="S11" t="s">
-        <v>222</v>
-      </c>
       <c r="T11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="U11" t="s">
         <v>210</v>
@@ -8673,22 +8673,22 @@
         <v>212</v>
       </c>
       <c r="X11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Y11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Z11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AA11" t="s">
         <v>212</v>
       </c>
       <c r="AB11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AC11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AD11" t="s">
         <v>212</v>
@@ -8703,22 +8703,22 @@
         <v>0.57692307692307687</v>
       </c>
       <c r="R12" t="s">
-        <v>221</v>
+        <v>478</v>
       </c>
       <c r="S12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="T12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="U12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="V12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="W12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="X12" t="s">
         <v>214</v>
@@ -8733,10 +8733,10 @@
         <v>216</v>
       </c>
       <c r="AB12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AC12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AD12" t="s">
         <v>216</v>
@@ -8754,43 +8754,43 @@
         <v>59</v>
       </c>
       <c r="R13" t="s">
-        <v>223</v>
+        <v>479</v>
       </c>
       <c r="S13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="T13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="U13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="V13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="W13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="X13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Y13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Z13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AA13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AB13" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="AC13" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="AD13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -8807,7 +8807,7 @@
         <v>184</v>
       </c>
       <c r="S14" s="1">
-        <f t="shared" ref="S14:AD14" si="2">$R$5</f>
+        <f t="shared" ref="S14:AE14" si="2">$R$5</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="T14" s="1">
@@ -8854,22 +8854,23 @@
         <f t="shared" si="2"/>
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="AE14" s="1"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B15">
         <v>3.9</v>
       </c>
       <c r="C15" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="R15" t="s">
         <v>189</v>
       </c>
       <c r="S15" s="2">
-        <f t="shared" ref="S15:AD15" si="3">$S$5</f>
+        <f t="shared" ref="S15:AE15" si="3">$S$5</f>
         <v>8.5810517220665614E-2</v>
       </c>
       <c r="T15" s="2">
@@ -8916,6 +8917,7 @@
         <f t="shared" si="3"/>
         <v>8.5810517220665614E-2</v>
       </c>
+      <c r="AE15" s="2"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -8928,7 +8930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -8943,7 +8945,7 @@
         <v>60</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" ref="S17:AD17" si="4">$Y$4</f>
+        <f t="shared" ref="S17:AE17" si="4">$Y$4</f>
         <v>678.26769230769241</v>
       </c>
       <c r="T17" s="5">
@@ -8990,8 +8992,9 @@
         <f t="shared" si="4"/>
         <v>678.26769230769241</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE17" s="5"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -9006,7 +9009,7 @@
         <v>58</v>
       </c>
       <c r="S18">
-        <f t="shared" ref="S18:AD18" si="5">$AC$5</f>
+        <f t="shared" ref="S18:AE18" si="5">$AC$5</f>
         <v>10</v>
       </c>
       <c r="T18">
@@ -9054,7 +9057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>165</v>
       </c>
@@ -9066,7 +9069,7 @@
         <v>20</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" ref="S19:AD19" si="6">S$17*S$15+$B$32</f>
+        <f t="shared" ref="S19:AE19" si="6">S$17*S$15+$B$32</f>
         <v>65.002501490990369</v>
       </c>
       <c r="T19" s="5">
@@ -9113,8 +9116,9 @@
         <f t="shared" si="6"/>
         <v>65.002501490990369</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE19" s="5"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -9129,7 +9133,7 @@
         <v>32</v>
       </c>
       <c r="S20" s="5">
-        <f t="shared" ref="S20:AD20" si="7">($B$34*S$18*10^-3 + $B$33)/(1-$B$46)</f>
+        <f t="shared" ref="S20:AE20" si="7">($B$34*S$18*10^-3 + $B$33)/(1-$B$46)</f>
         <v>126.97417171717171</v>
       </c>
       <c r="T20" s="5">
@@ -9176,8 +9180,9 @@
         <f t="shared" si="7"/>
         <v>126.97417171717171</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE20" s="5"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -9189,7 +9194,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -9204,7 +9209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -9222,7 +9227,7 @@
         <v>61</v>
       </c>
       <c r="S23" s="5">
-        <f t="shared" ref="S23:AD23" si="8">$AA$4</f>
+        <f t="shared" ref="S23:AE23" si="8">$AA$4</f>
         <v>775.16307692307703</v>
       </c>
       <c r="T23" s="5">
@@ -9269,8 +9274,9 @@
         <f t="shared" si="8"/>
         <v>775.16307692307703</v>
       </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE23" s="5"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -9285,7 +9291,7 @@
         <v>20</v>
       </c>
       <c r="S24" s="5">
-        <f t="shared" ref="S24:AD24" si="9">S$23*S$15+$C$32</f>
+        <f t="shared" ref="S24:AE24" si="9">S$23*S$15+$C$32</f>
         <v>77.517144561131843</v>
       </c>
       <c r="T24" s="5">
@@ -9332,8 +9338,9 @@
         <f t="shared" si="9"/>
         <v>77.517144561131843</v>
       </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE24" s="5"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -9347,7 +9354,7 @@
         <v>32</v>
       </c>
       <c r="S25" s="5">
-        <f t="shared" ref="S25:AD25" si="10">($C$34*S$18*10^-3 + $C$33)/(1-$C$46)</f>
+        <f t="shared" ref="S25:AE25" si="10">($C$34*S$18*10^-3 + $C$33)/(1-$C$46)</f>
         <v>84.936820512820518</v>
       </c>
       <c r="T25" s="5">
@@ -9394,8 +9401,9 @@
         <f t="shared" si="10"/>
         <v>84.936820512820518</v>
       </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE25" s="5"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -9406,12 +9414,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="R27" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -9466,11 +9474,12 @@
         <v>976.42784318082204</v>
       </c>
       <c r="AD28" s="5">
-        <f t="shared" ref="AD28" si="12">INDEX($T$4:$U$5, MATCH(AD10,$T$4:$T$5),2)</f>
+        <f t="shared" ref="AD28:AE28" si="12">INDEX($T$4:$U$5, MATCH(AD10,$T$4:$T$5),2)</f>
         <v>1140</v>
       </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE28" s="5"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
@@ -9481,7 +9490,7 @@
         <v>183</v>
       </c>
       <c r="S29" s="4">
-        <f t="shared" ref="S29:AC29" si="13">$W$4</f>
+        <f t="shared" ref="S29:AE29" si="13">$W$4</f>
         <v>2.6153846153846154</v>
       </c>
       <c r="T29" s="4">
@@ -9528,8 +9537,9 @@
         <f>$W$5</f>
         <v>3.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE29" s="4"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>1</v>
       </c>
@@ -9555,7 +9565,7 @@
         <v>20</v>
       </c>
       <c r="S30" s="5">
-        <f t="shared" ref="S30:AD30" si="14">S$28*S$15+$D$32</f>
+        <f t="shared" ref="S30:AE30" si="14">S$28*S$15+$D$32</f>
         <v>125.88777825200532</v>
       </c>
       <c r="T30" s="5">
@@ -9602,8 +9612,9 @@
         <f t="shared" si="14"/>
         <v>139.92398963155881</v>
       </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE30" s="5"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -9638,7 +9649,7 @@
         <v>32</v>
       </c>
       <c r="S31" s="5">
-        <f t="shared" ref="S31:AD31" si="16">($D$34*S$29*$E$3*10^-3 + $D$33)/(1-$D$46)</f>
+        <f t="shared" ref="S31:AE31" si="16">($D$34*S$29*$E$3*10^-3 + $D$33)/(1-$D$46)</f>
         <v>32.466607822649564</v>
       </c>
       <c r="T31" s="5">
@@ -9685,8 +9696,9 @@
         <f t="shared" si="16"/>
         <v>45.902984148611111</v>
       </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE31" s="5"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -9718,7 +9730,7 @@
         <v>2736.5</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -9754,7 +9766,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -9777,7 +9789,7 @@
         <v>75</v>
       </c>
       <c r="Q34" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="R34" t="s">
         <v>55</v>
@@ -9827,11 +9839,12 @@
         <v>3.3984353954038309E-2</v>
       </c>
       <c r="AD34" s="2">
-        <f t="shared" ref="AD34" si="18">(AD24-AD19)*1000/(AD20-AD25)/8760</f>
+        <f t="shared" ref="AD34:AE34" si="18">(AD24-AD19)*1000/(AD20-AD25)/8760</f>
         <v>3.3984353954038309E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE34" s="2"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -9901,11 +9914,12 @@
         <v>0.10523612453151106</v>
       </c>
       <c r="AD35" s="2">
-        <f t="shared" ref="AD35" si="20">(AD30-AD24)*1000/(AD25-AD31)/8760</f>
+        <f t="shared" ref="AD35:AE35" si="20">(AD30-AD24)*1000/(AD25-AD31)/8760</f>
         <v>0.18251009215426989</v>
       </c>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE35" s="2"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>166</v>
       </c>
@@ -9961,7 +9975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -10030,7 +10044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -10098,8 +10112,9 @@
         <f t="shared" si="22"/>
         <v>678.26769230769241</v>
       </c>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE38" s="5"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -10167,8 +10182,9 @@
         <f t="shared" si="23"/>
         <v>775.16307692307703</v>
       </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE39" s="5"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -10240,8 +10256,9 @@
         <f t="shared" si="24"/>
         <v>1140</v>
       </c>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE40" s="5"/>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -10262,7 +10279,7 @@
         <v>551.69230769230774</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -10285,7 +10302,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -10308,7 +10325,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -10378,8 +10395,9 @@
         <f t="shared" si="26"/>
         <v>65.002501490990369</v>
       </c>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE44" s="5"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -10449,8 +10467,9 @@
         <f t="shared" si="27"/>
         <v>1177.2962457334145</v>
       </c>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE45" s="5"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -10520,8 +10539,9 @@
         <f t="shared" si="28"/>
         <v>77.517144561131843</v>
       </c>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE46" s="5"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Q47">
         <v>8760</v>
       </c>
@@ -10576,8 +10596,9 @@
         <f t="shared" si="29"/>
         <v>821.56369225343963</v>
       </c>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE47" s="5"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -10649,8 +10670,9 @@
         <f t="shared" si="30"/>
         <v>139.92398963155881</v>
       </c>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE48" s="5"/>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -10720,8 +10742,9 @@
         <f t="shared" si="31"/>
         <v>542.03413077339212</v>
       </c>
-    </row>
-    <row r="50" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE49" s="5"/>
+    </row>
+    <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -10738,7 +10761,7 @@
         <v>8.5810517220665614E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -10755,13 +10778,13 @@
         <v>125.88777825200532</v>
       </c>
       <c r="Q51" s="20" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="R51" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -10847,7 +10870,7 @@
         <v>coalhcW30lcS30lc</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -10926,8 +10949,9 @@
         <f t="shared" si="33"/>
         <v>678.26769230769241</v>
       </c>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE53" s="5"/>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -10965,7 +10989,7 @@
         <v>199</v>
       </c>
       <c r="S54" s="4">
-        <f t="shared" ref="S54:AD54" si="34">$B$32</f>
+        <f t="shared" ref="S54:AE54" si="34">$B$32</f>
         <v>6.8</v>
       </c>
       <c r="T54" s="4">
@@ -11012,8 +11036,9 @@
         <f t="shared" si="34"/>
         <v>6.8</v>
       </c>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE54" s="4"/>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -11094,8 +11119,9 @@
         <f t="shared" si="35"/>
         <v>775.16307692307703</v>
       </c>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE55" s="5"/>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>191</v>
       </c>
@@ -11110,7 +11136,7 @@
         <v>200</v>
       </c>
       <c r="S56" s="4">
-        <f t="shared" ref="S56:AD56" si="36">$C$32</f>
+        <f t="shared" ref="S56:AE56" si="36">$C$32</f>
         <v>11</v>
       </c>
       <c r="T56" s="4">
@@ -11157,8 +11183,9 @@
         <f t="shared" si="36"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE56" s="4"/>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="Q57" t="s">
         <v>203</v>
@@ -11214,8 +11241,9 @@
         <f t="shared" si="37"/>
         <v>1140</v>
       </c>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE57" s="5"/>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="Q58" t="s">
         <v>204</v>
@@ -11224,7 +11252,7 @@
         <v>57</v>
       </c>
       <c r="S58" s="4">
-        <f t="shared" ref="S58:AD58" si="38">$D$32</f>
+        <f t="shared" ref="S58:AE58" si="38">$D$32</f>
         <v>42.1</v>
       </c>
       <c r="T58" s="4">
@@ -11271,8 +11299,9 @@
         <f t="shared" si="38"/>
         <v>42.1</v>
       </c>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE58" s="4"/>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>149</v>
       </c>
@@ -11331,7 +11360,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>147</v>
       </c>
@@ -11390,7 +11419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0</v>
       </c>
@@ -11461,7 +11490,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>8760</v>
       </c>
@@ -11532,7 +11561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -11552,7 +11581,7 @@
         <v>203</v>
       </c>
       <c r="R63" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="S63">
         <f t="shared" ref="S63:AD63" si="43">INDEX($AJ$4:$AL$7, MATCH(S13,$AJ$4:$AJ$7,0), 2)</f>
@@ -11603,12 +11632,12 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Q64" t="s">
         <v>204</v>
       </c>
       <c r="R64" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="S64">
         <f t="shared" ref="S64:AD64" si="44">INDEX($AJ$4:$AL$7, MATCH(S13,$AJ$4:$AJ$7,0), 3)</f>
@@ -11661,7 +11690,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -11674,7 +11703,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B68">
         <v>1100</v>
@@ -11685,7 +11714,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B69">
         <v>15</v>
@@ -11696,7 +11725,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B70" s="1">
         <v>0.28000000000000003</v>
@@ -11733,7 +11762,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B73">
         <v>2.4300000000000002</v>
@@ -11758,15 +11787,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -13509,7 +13543,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -13518,12 +13552,12 @@
       </c>
       <c r="E18" s="5"/>
       <c r="H18" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -13533,7 +13567,7 @@
       </c>
       <c r="E19" s="5"/>
       <c r="H19" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -14882,47 +14916,47 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -14930,7 +14964,7 @@
         <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -14938,7 +14972,7 @@
         <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -14946,7 +14980,7 @@
         <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -14954,7 +14988,7 @@
         <v>200</v>
       </c>
       <c r="C9" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -14962,7 +14996,7 @@
         <v>200</v>
       </c>
       <c r="C10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -14970,7 +15004,7 @@
         <v>300</v>
       </c>
       <c r="C11" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -14978,7 +15012,7 @@
         <v>300</v>
       </c>
       <c r="C12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -14986,7 +15020,7 @@
         <v>300</v>
       </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -14994,7 +15028,7 @@
         <v>300</v>
       </c>
       <c r="C14" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -15002,7 +15036,7 @@
         <v>300</v>
       </c>
       <c r="C15" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -15010,7 +15044,7 @@
         <v>400</v>
       </c>
       <c r="C16" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -15018,7 +15052,7 @@
         <v>400</v>
       </c>
       <c r="C17" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -15026,7 +15060,7 @@
         <v>400</v>
       </c>
       <c r="C18" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -15034,7 +15068,7 @@
         <v>400</v>
       </c>
       <c r="C19" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -15042,442 +15076,442 @@
         <v>400</v>
       </c>
       <c r="C20" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G24" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G25" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H25" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I25" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E26" s="7" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G26" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H26" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G27" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H27" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G28" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H28" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G29" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H29" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="H30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D31" s="7" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G31" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H31" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I31" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D32" s="7" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G32" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="H32" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I32" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" s="7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G33" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="I33" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" s="22" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G34" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H34" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I34" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G35" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H35" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I35" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G36" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="H36" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I36" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" s="7" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G37" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H37" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I37" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I38" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="I39" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F40" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I40" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F41" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I41" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G42" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I43" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I44" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G45" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D46" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G46" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D47" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G47" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G48" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G49" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E54" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F54" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G54" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E55" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F55" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G55" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E56" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G56" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E63" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F63" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E64" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F64" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E65" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F65" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
+        <v>316</v>
+      </c>
+      <c r="E66" t="s">
         <v>319</v>
       </c>
-      <c r="E66" t="s">
-        <v>322</v>
-      </c>
       <c r="F66" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F67" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F68" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F69" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F70" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F71" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the scenario economic dispatch name for 0 min gen - removed G0
</commit_message>
<xml_diff>
--- a/india_REV_input/Scenarios_Cost_Master_v4.xlsx
+++ b/india_REV_input/Scenarios_Cost_Master_v4.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Electricity_Models\renewable_energy_value\india_REV_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ranjitster/Dropbox/renewable_energy_value/renewable_energy_value/india_REV_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30495" yWindow="-3600" windowWidth="25035" windowHeight="14955" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25040" windowHeight="14960"/>
   </bookViews>
   <sheets>
     <sheet name="REvalue_input_csv" sheetId="11" r:id="rId1"/>
@@ -23,13 +23,16 @@
     <sheet name="scenarios" sheetId="13" r:id="rId9"/>
     <sheet name="run_times" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -42,7 +45,7 @@
     <author>Ranjit Deshmukh</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="1" shapeId="0">
+    <comment ref="D6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -102,7 +105,7 @@
     <author>Ranjit</author>
   </authors>
   <commentList>
-    <comment ref="AC5" authorId="0" shapeId="0">
+    <comment ref="AC5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="1" shapeId="0">
+    <comment ref="B6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -152,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="1" shapeId="0">
+    <comment ref="A8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -176,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="1" shapeId="0">
+    <comment ref="B16" authorId="1">
       <text>
         <r>
           <rPr>
@@ -201,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="1" shapeId="0">
+    <comment ref="B18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -225,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="1" shapeId="0">
+    <comment ref="D34" authorId="1">
       <text>
         <r>
           <rPr>
@@ -250,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="1" shapeId="0">
+    <comment ref="B37" authorId="1">
       <text>
         <r>
           <rPr>
@@ -274,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="1" shapeId="0">
+    <comment ref="D37" authorId="1">
       <text>
         <r>
           <rPr>
@@ -308,7 +311,7 @@
     <author>Ranjit</author>
   </authors>
   <commentList>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -333,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0">
+    <comment ref="C22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0">
+    <comment ref="D22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -382,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0">
+    <comment ref="E22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -407,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="0" shapeId="0">
+    <comment ref="E34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B61" authorId="0" shapeId="0">
+    <comment ref="B61" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2412,38 +2415,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="R8" sqref="R8"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>225</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>243</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>ClcC70mLmod_D25_M25_energyOnly</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>245</v>
       </c>
@@ -2772,7 +2775,7 @@
         <v>ClcC70mLmod_D25_M25_energyOnly</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>413</v>
       </c>
@@ -2789,8 +2792,8 @@
         <v>ClcC55m</v>
       </c>
       <c r="F4" t="str">
-        <f>CONCATENATE(F10,F13,F15,F17,F19,F21,F36,F39,F42,F44,F47)</f>
-        <v>ClcC0mG0m</v>
+        <f>CONCATENATE(F10,F13,F17,F19,F21,F36,F39,F42,F44,F47)</f>
+        <v>ClcC0m</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ref="G4:AD4" si="5">CONCATENATE(G10,G13,G15,G17,G19,G21,G36,G39,G42,G44,G47)</f>
@@ -2889,7 +2892,7 @@
         <v>ClcC70mLmod_D25_M25_energyOnly</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>246</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>coallcLmod_D25_M25_energyOnly</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3123,7 +3126,7 @@
         <v>coallcLmod_D25_M25_energyOnly</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>248</v>
       </c>
@@ -3240,7 +3243,7 @@
         <v>W80_S0d</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>249</v>
       </c>
@@ -3357,7 +3360,7 @@
         <v>coallc</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>250</v>
       </c>
@@ -3449,7 +3452,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>254</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>Clc</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>255</v>
       </c>
@@ -3683,7 +3686,7 @@
         <v>coallc</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>256</v>
       </c>
@@ -3775,7 +3778,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>258</v>
       </c>
@@ -3792,7 +3795,7 @@
         <v>C55m</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" ref="F13:U15" si="24">CONCATENATE("C",F12,"m")</f>
+        <f t="shared" ref="F13" si="24">CONCATENATE("C",F12,"m")</f>
         <v>C0m</v>
       </c>
       <c r="G13" t="str">
@@ -3876,7 +3879,7 @@
         <v>C70m</v>
       </c>
       <c r="AA13" t="str">
-        <f t="shared" ref="AA13:AA15" si="25">CONCATENATE("C",AA12,"m")</f>
+        <f t="shared" ref="AA13" si="25">CONCATENATE("C",AA12,"m")</f>
         <v>C70m</v>
       </c>
       <c r="AB13" t="str">
@@ -3892,7 +3895,7 @@
         <v>C70m</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>474</v>
       </c>
@@ -3984,7 +3987,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>475</v>
       </c>
@@ -4101,7 +4104,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>259</v>
       </c>
@@ -4193,12 +4196,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>261</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" ref="C15:U17" si="27">IF(C16=0,"",CONCATENATE("H",C16))</f>
+        <f t="shared" ref="C17:U17" si="27">IF(C16=0,"",CONCATENATE("H",C16))</f>
         <v/>
       </c>
       <c r="D17" t="str">
@@ -4310,7 +4313,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>262</v>
       </c>
@@ -4402,7 +4405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>264</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>265</v>
       </c>
@@ -4611,7 +4614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>267</v>
       </c>
@@ -4728,7 +4731,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>268</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>bat0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>415</v>
       </c>
@@ -4937,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>416</v>
       </c>
@@ -5029,7 +5032,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>417</v>
       </c>
@@ -5146,7 +5149,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>418</v>
       </c>
@@ -5263,7 +5266,7 @@
         <v>batteryLC0</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>269</v>
       </c>
@@ -5355,7 +5358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>271</v>
       </c>
@@ -5447,7 +5450,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>273</v>
       </c>
@@ -5564,7 +5567,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>274</v>
       </c>
@@ -5681,7 +5684,7 @@
         <v>windLC0</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
         <v>275</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>276</v>
       </c>
@@ -5865,7 +5868,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>277</v>
       </c>
@@ -5982,7 +5985,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>278</v>
       </c>
@@ -6099,7 +6102,7 @@
         <v>solarLC0</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>279</v>
       </c>
@@ -6191,7 +6194,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>281</v>
       </c>
@@ -6308,7 +6311,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>282</v>
       </c>
@@ -6425,7 +6428,7 @@
         <v>W80</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>283</v>
       </c>
@@ -6517,7 +6520,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>288</v>
       </c>
@@ -6634,7 +6637,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>289</v>
       </c>
@@ -6751,7 +6754,7 @@
         <v>S0d</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>290</v>
       </c>
@@ -6841,7 +6844,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>291</v>
       </c>
@@ -6958,7 +6961,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>292</v>
       </c>
@@ -7050,7 +7053,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>295</v>
       </c>
@@ -7167,7 +7170,7 @@
         <v>Lmod_D25_M25_energyOnly</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
         <v>296</v>
       </c>
@@ -7259,7 +7262,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>299</v>
       </c>
@@ -7348,7 +7351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>300</v>
       </c>
@@ -7469,11 +7472,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7485,13 +7483,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>312</v>
       </c>
@@ -7502,7 +7500,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>309</v>
       </c>
@@ -7519,7 +7517,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>303</v>
       </c>
@@ -7544,7 +7542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>303</v>
       </c>
@@ -7569,7 +7567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>303</v>
       </c>
@@ -7588,7 +7586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>303</v>
       </c>
@@ -7616,11 +7614,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7632,31 +7625,31 @@
       <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>220</v>
       </c>
@@ -7739,7 +7732,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>439</v>
       </c>
@@ -7822,7 +7815,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>409</v>
       </c>
@@ -7908,7 +7901,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>410</v>
       </c>
@@ -7994,7 +7987,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>406</v>
       </c>
@@ -8053,7 +8046,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>407</v>
       </c>
@@ -8112,7 +8105,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>408</v>
       </c>
@@ -8174,11 +8167,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8190,36 +8178,36 @@
       <selection activeCell="AE9" sqref="AE9:AE64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" customWidth="1"/>
-    <col min="21" max="21" width="24.42578125" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="24.5" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" customWidth="1"/>
-    <col min="25" max="25" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" customWidth="1"/>
-    <col min="27" max="27" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" customWidth="1"/>
+    <col min="25" max="25" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5" customWidth="1"/>
+    <col min="27" max="27" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.5" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="28" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -8233,7 +8221,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>35</v>
       </c>
@@ -8241,7 +8229,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>34</v>
       </c>
@@ -8288,7 +8276,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>54</v>
       </c>
@@ -8372,7 +8360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -8446,7 +8434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -8496,7 +8484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -8527,7 +8515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -8538,7 +8526,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -8598,7 +8586,7 @@
         <v>coalhcW30lcS30lc</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8646,7 +8634,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8694,7 +8682,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -8742,7 +8730,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -8793,7 +8781,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -8807,7 +8795,7 @@
         <v>184</v>
       </c>
       <c r="S14" s="1">
-        <f t="shared" ref="S14:AE14" si="2">$R$5</f>
+        <f t="shared" ref="S14:AD14" si="2">$R$5</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="T14" s="1">
@@ -8856,7 +8844,7 @@
       </c>
       <c r="AE14" s="1"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>434</v>
       </c>
@@ -8870,7 +8858,7 @@
         <v>189</v>
       </c>
       <c r="S15" s="2">
-        <f t="shared" ref="S15:AE15" si="3">$S$5</f>
+        <f t="shared" ref="S15:AD15" si="3">$S$5</f>
         <v>8.5810517220665614E-2</v>
       </c>
       <c r="T15" s="2">
@@ -8919,7 +8907,7 @@
       </c>
       <c r="AE15" s="2"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -8930,7 +8918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -8945,7 +8933,7 @@
         <v>60</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" ref="S17:AE17" si="4">$Y$4</f>
+        <f t="shared" ref="S17:AD17" si="4">$Y$4</f>
         <v>678.26769230769241</v>
       </c>
       <c r="T17" s="5">
@@ -8994,7 +8982,7 @@
       </c>
       <c r="AE17" s="5"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -9009,7 +8997,7 @@
         <v>58</v>
       </c>
       <c r="S18">
-        <f t="shared" ref="S18:AE18" si="5">$AC$5</f>
+        <f t="shared" ref="S18:AD18" si="5">$AC$5</f>
         <v>10</v>
       </c>
       <c r="T18">
@@ -9057,7 +9045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>165</v>
       </c>
@@ -9069,7 +9057,7 @@
         <v>20</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" ref="S19:AE19" si="6">S$17*S$15+$B$32</f>
+        <f t="shared" ref="S19:AD19" si="6">S$17*S$15+$B$32</f>
         <v>65.002501490990369</v>
       </c>
       <c r="T19" s="5">
@@ -9118,7 +9106,7 @@
       </c>
       <c r="AE19" s="5"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -9133,7 +9121,7 @@
         <v>32</v>
       </c>
       <c r="S20" s="5">
-        <f t="shared" ref="S20:AE20" si="7">($B$34*S$18*10^-3 + $B$33)/(1-$B$46)</f>
+        <f t="shared" ref="S20:AD20" si="7">($B$34*S$18*10^-3 + $B$33)/(1-$B$46)</f>
         <v>126.97417171717171</v>
       </c>
       <c r="T20" s="5">
@@ -9182,7 +9170,7 @@
       </c>
       <c r="AE20" s="5"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -9194,7 +9182,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -9209,7 +9197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -9227,7 +9215,7 @@
         <v>61</v>
       </c>
       <c r="S23" s="5">
-        <f t="shared" ref="S23:AE23" si="8">$AA$4</f>
+        <f t="shared" ref="S23:AD23" si="8">$AA$4</f>
         <v>775.16307692307703</v>
       </c>
       <c r="T23" s="5">
@@ -9276,7 +9264,7 @@
       </c>
       <c r="AE23" s="5"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -9291,7 +9279,7 @@
         <v>20</v>
       </c>
       <c r="S24" s="5">
-        <f t="shared" ref="S24:AE24" si="9">S$23*S$15+$C$32</f>
+        <f t="shared" ref="S24:AD24" si="9">S$23*S$15+$C$32</f>
         <v>77.517144561131843</v>
       </c>
       <c r="T24" s="5">
@@ -9340,7 +9328,7 @@
       </c>
       <c r="AE24" s="5"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -9354,7 +9342,7 @@
         <v>32</v>
       </c>
       <c r="S25" s="5">
-        <f t="shared" ref="S25:AE25" si="10">($C$34*S$18*10^-3 + $C$33)/(1-$C$46)</f>
+        <f t="shared" ref="S25:AD25" si="10">($C$34*S$18*10^-3 + $C$33)/(1-$C$46)</f>
         <v>84.936820512820518</v>
       </c>
       <c r="T25" s="5">
@@ -9403,7 +9391,7 @@
       </c>
       <c r="AE25" s="5"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -9414,12 +9402,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="R27" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -9474,12 +9462,12 @@
         <v>976.42784318082204</v>
       </c>
       <c r="AD28" s="5">
-        <f t="shared" ref="AD28:AE28" si="12">INDEX($T$4:$U$5, MATCH(AD10,$T$4:$T$5),2)</f>
+        <f t="shared" ref="AD28" si="12">INDEX($T$4:$U$5, MATCH(AD10,$T$4:$T$5),2)</f>
         <v>1140</v>
       </c>
       <c r="AE28" s="5"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
@@ -9490,7 +9478,7 @@
         <v>183</v>
       </c>
       <c r="S29" s="4">
-        <f t="shared" ref="S29:AE29" si="13">$W$4</f>
+        <f t="shared" ref="S29:AC29" si="13">$W$4</f>
         <v>2.6153846153846154</v>
       </c>
       <c r="T29" s="4">
@@ -9539,7 +9527,7 @@
       </c>
       <c r="AE29" s="4"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>1</v>
       </c>
@@ -9565,7 +9553,7 @@
         <v>20</v>
       </c>
       <c r="S30" s="5">
-        <f t="shared" ref="S30:AE30" si="14">S$28*S$15+$D$32</f>
+        <f t="shared" ref="S30:AD30" si="14">S$28*S$15+$D$32</f>
         <v>125.88777825200532</v>
       </c>
       <c r="T30" s="5">
@@ -9614,7 +9602,7 @@
       </c>
       <c r="AE30" s="5"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -9649,7 +9637,7 @@
         <v>32</v>
       </c>
       <c r="S31" s="5">
-        <f t="shared" ref="S31:AE31" si="16">($D$34*S$29*$E$3*10^-3 + $D$33)/(1-$D$46)</f>
+        <f t="shared" ref="S31:AD31" si="16">($D$34*S$29*$E$3*10^-3 + $D$33)/(1-$D$46)</f>
         <v>32.466607822649564</v>
       </c>
       <c r="T31" s="5">
@@ -9698,7 +9686,7 @@
       </c>
       <c r="AE31" s="5"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -9730,7 +9718,7 @@
         <v>2736.5</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -9766,7 +9754,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -9839,12 +9827,12 @@
         <v>3.3984353954038309E-2</v>
       </c>
       <c r="AD34" s="2">
-        <f t="shared" ref="AD34:AE34" si="18">(AD24-AD19)*1000/(AD20-AD25)/8760</f>
+        <f t="shared" ref="AD34" si="18">(AD24-AD19)*1000/(AD20-AD25)/8760</f>
         <v>3.3984353954038309E-2</v>
       </c>
       <c r="AE34" s="2"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -9914,12 +9902,12 @@
         <v>0.10523612453151106</v>
       </c>
       <c r="AD35" s="2">
-        <f t="shared" ref="AD35:AE35" si="20">(AD30-AD24)*1000/(AD25-AD31)/8760</f>
+        <f t="shared" ref="AD35" si="20">(AD30-AD24)*1000/(AD25-AD31)/8760</f>
         <v>0.18251009215426989</v>
       </c>
       <c r="AE35" s="2"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>166</v>
       </c>
@@ -9975,7 +9963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -10044,7 +10032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -10114,7 +10102,7 @@
       </c>
       <c r="AE38" s="5"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -10184,7 +10172,7 @@
       </c>
       <c r="AE39" s="5"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -10258,7 +10246,7 @@
       </c>
       <c r="AE40" s="5"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -10279,7 +10267,7 @@
         <v>551.69230769230774</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -10302,7 +10290,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -10325,7 +10313,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -10397,7 +10385,7 @@
       </c>
       <c r="AE44" s="5"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -10469,7 +10457,7 @@
       </c>
       <c r="AE45" s="5"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -10541,7 +10529,7 @@
       </c>
       <c r="AE46" s="5"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="Q47">
         <v>8760</v>
       </c>
@@ -10598,7 +10586,7 @@
       </c>
       <c r="AE47" s="5"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -10672,7 +10660,7 @@
       </c>
       <c r="AE48" s="5"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -10744,7 +10732,7 @@
       </c>
       <c r="AE49" s="5"/>
     </row>
-    <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -10761,7 +10749,7 @@
         <v>8.5810517220665614E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -10784,7 +10772,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -10870,7 +10858,7 @@
         <v>coalhcW30lcS30lc</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -10951,7 +10939,7 @@
       </c>
       <c r="AE53" s="5"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -10989,7 +10977,7 @@
         <v>199</v>
       </c>
       <c r="S54" s="4">
-        <f t="shared" ref="S54:AE54" si="34">$B$32</f>
+        <f t="shared" ref="S54:AD54" si="34">$B$32</f>
         <v>6.8</v>
       </c>
       <c r="T54" s="4">
@@ -11038,7 +11026,7 @@
       </c>
       <c r="AE54" s="4"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -11121,7 +11109,7 @@
       </c>
       <c r="AE55" s="5"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>191</v>
       </c>
@@ -11136,7 +11124,7 @@
         <v>200</v>
       </c>
       <c r="S56" s="4">
-        <f t="shared" ref="S56:AE56" si="36">$C$32</f>
+        <f t="shared" ref="S56:AD56" si="36">$C$32</f>
         <v>11</v>
       </c>
       <c r="T56" s="4">
@@ -11185,7 +11173,7 @@
       </c>
       <c r="AE56" s="4"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B57" s="12"/>
       <c r="Q57" t="s">
         <v>203</v>
@@ -11243,7 +11231,7 @@
       </c>
       <c r="AE57" s="5"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B58" s="12"/>
       <c r="Q58" t="s">
         <v>204</v>
@@ -11252,7 +11240,7 @@
         <v>57</v>
       </c>
       <c r="S58" s="4">
-        <f t="shared" ref="S58:AE58" si="38">$D$32</f>
+        <f t="shared" ref="S58:AD58" si="38">$D$32</f>
         <v>42.1</v>
       </c>
       <c r="T58" s="4">
@@ -11301,7 +11289,7 @@
       </c>
       <c r="AE58" s="4"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>149</v>
       </c>
@@ -11360,7 +11348,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>147</v>
       </c>
@@ -11419,7 +11407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>0</v>
       </c>
@@ -11490,7 +11478,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>8760</v>
       </c>
@@ -11561,7 +11549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -11632,7 +11620,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.2">
       <c r="Q64" t="s">
         <v>204</v>
       </c>
@@ -11688,12 +11676,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>159</v>
       </c>
@@ -11701,7 +11689,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>427</v>
       </c>
@@ -11712,7 +11700,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>428</v>
       </c>
@@ -11723,7 +11711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>430</v>
       </c>
@@ -11734,7 +11722,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>153</v>
       </c>
@@ -11747,7 +11735,7 @@
         <v>44.890647132724027</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>155</v>
       </c>
@@ -11760,7 +11748,7 @@
         <v>2.917892063627062</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>429</v>
       </c>
@@ -11775,11 +11763,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11787,23 +11770,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>'Screening curves'!Q34</f>
         <v>parameter</v>
@@ -11857,7 +11840,7 @@
         <v>coalhcW30lcS30lc</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Screening curves'!R34</f>
         <v>gas_ct</v>
@@ -11915,7 +11898,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Screening curves'!R35</f>
         <v>gas_ccgt</v>
@@ -11973,7 +11956,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>'Screening curves'!R36</f>
         <v>coal</v>
@@ -12031,7 +12014,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>'Screening curves'!R37</f>
         <v>gas_price</v>
@@ -12089,7 +12072,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Screening curves'!R38</f>
         <v>cap_cost_ct</v>
@@ -12147,7 +12130,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Screening curves'!R39</f>
         <v>cap_cost_ccgt</v>
@@ -12205,7 +12188,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>'Screening curves'!R40</f>
         <v>cap_cost_coal</v>
@@ -12266,11 +12249,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12282,13 +12260,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>'Screening curves'!Q43</f>
         <v>hour</v>
@@ -12306,7 +12284,7 @@
         <v>coalhc</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>'Screening curves'!Q44</f>
         <v>0</v>
@@ -12324,7 +12302,7 @@
         <v>65.002501490990369</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>'Screening curves'!Q45</f>
         <v>8760</v>
@@ -12342,7 +12320,7 @@
         <v>1177.2962457334145</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>'Screening curves'!Q46</f>
         <v>0</v>
@@ -12360,7 +12338,7 @@
         <v>77.517144561131843</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>'Screening curves'!Q47</f>
         <v>8760</v>
@@ -12378,7 +12356,7 @@
         <v>821.56369225343963</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>'Screening curves'!Q48</f>
         <v>0</v>
@@ -12396,7 +12374,7 @@
         <v>139.92398963155881</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>'Screening curves'!Q49</f>
         <v>8760</v>
@@ -12416,11 +12394,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12432,20 +12405,20 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>'Screening curves'!Q52</f>
         <v>cost_type</v>
@@ -12503,7 +12476,7 @@
         <v>coalhcW30lcS30lc</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Screening curves'!Q53</f>
         <v>capital</v>
@@ -12561,7 +12534,7 @@
         <v>678.26769230769241</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Screening curves'!Q54</f>
         <v>om</v>
@@ -12619,7 +12592,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>'Screening curves'!Q55</f>
         <v>capital</v>
@@ -12677,7 +12650,7 @@
         <v>775.16307692307703</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>'Screening curves'!Q56</f>
         <v>om</v>
@@ -12735,7 +12708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Screening curves'!Q57</f>
         <v>capital</v>
@@ -12793,7 +12766,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Screening curves'!Q58</f>
         <v>om</v>
@@ -12851,7 +12824,7 @@
         <v>42.1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>'Screening curves'!Q59</f>
         <v>capital</v>
@@ -12909,7 +12882,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>'Screening curves'!Q60</f>
         <v>om</v>
@@ -12967,7 +12940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'Screening curves'!Q61</f>
         <v>capital</v>
@@ -13025,7 +12998,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>'Screening curves'!Q62</f>
         <v>om</v>
@@ -13083,7 +13056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>'Screening curves'!Q63</f>
         <v>capital</v>
@@ -13141,7 +13114,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>'Screening curves'!Q64</f>
         <v>om</v>
@@ -13202,11 +13175,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13218,17 +13186,17 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -13251,12 +13219,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -13276,7 +13244,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -13301,7 +13269,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -13324,7 +13292,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -13353,7 +13321,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -13373,7 +13341,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -13397,7 +13365,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -13421,7 +13389,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -13441,7 +13409,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -13465,7 +13433,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -13489,7 +13457,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -13505,7 +13473,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -13523,7 +13491,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -13541,7 +13509,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>432</v>
       </c>
@@ -13555,7 +13523,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>432</v>
       </c>
@@ -13570,12 +13538,12 @@
         <v>433</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -13595,7 +13563,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -13621,7 +13589,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -13643,7 +13611,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -13665,7 +13633,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -13685,7 +13653,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -13702,7 +13670,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -13725,7 +13693,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -13748,7 +13716,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -13777,7 +13745,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>123</v>
       </c>
@@ -13806,12 +13774,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -13822,7 +13790,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -13836,7 +13804,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -13856,7 +13824,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -13873,7 +13841,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>95</v>
       </c>
@@ -13894,7 +13862,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -13914,7 +13882,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -13935,17 +13903,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>136</v>
       </c>
@@ -13956,7 +13924,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="8">
         <v>0.108</v>
       </c>
@@ -13964,12 +13932,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -13980,7 +13948,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>8.5</v>
       </c>
@@ -13988,7 +13956,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="7">
         <v>10</v>
       </c>
@@ -13996,7 +13964,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>5.5</v>
       </c>
@@ -14004,17 +13972,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>150</v>
       </c>
@@ -14025,7 +13993,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>151</v>
       </c>
@@ -14038,7 +14006,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>152</v>
       </c>
@@ -14050,7 +14018,7 @@
       </c>
       <c r="D61" s="17"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>162</v>
       </c>
@@ -14064,7 +14032,7 @@
       </c>
       <c r="D62" s="17"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -14076,7 +14044,7 @@
       </c>
       <c r="D63" s="18"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>156</v>
       </c>
@@ -14088,7 +14056,7 @@
       </c>
       <c r="D64" s="19"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -14102,7 +14070,7 @@
       </c>
       <c r="D65" s="9"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>157</v>
       </c>
@@ -14114,7 +14082,7 @@
       </c>
       <c r="D66" s="16"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>158</v>
       </c>
@@ -14126,7 +14094,7 @@
       </c>
       <c r="D67" s="16"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -14140,7 +14108,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -14154,7 +14122,7 @@
       </c>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -14172,11 +14140,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14188,40 +14151,40 @@
       <selection activeCell="B14" sqref="B14:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
         <v>107</v>
       </c>
@@ -14256,7 +14219,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -14268,7 +14231,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -14283,7 +14246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -14302,7 +14265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -14325,7 +14288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -14352,7 +14315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -14383,7 +14346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -14418,7 +14381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -14457,7 +14420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -14500,7 +14463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2017</v>
       </c>
@@ -14547,17 +14510,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="B22" s="13" t="s">
         <v>107</v>
       </c>
@@ -14592,7 +14555,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2008</v>
       </c>
@@ -14604,7 +14567,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2009</v>
       </c>
@@ -14619,7 +14582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2010</v>
       </c>
@@ -14638,7 +14601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2011</v>
       </c>
@@ -14661,7 +14624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2012</v>
       </c>
@@ -14688,7 +14651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2013</v>
       </c>
@@ -14719,7 +14682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2014</v>
       </c>
@@ -14754,7 +14717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2015</v>
       </c>
@@ -14793,7 +14756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2016</v>
       </c>
@@ -14836,7 +14799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2017</v>
       </c>
@@ -14885,11 +14848,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14901,25 +14859,25 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" customWidth="1"/>
+    <col min="9" max="9" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>403</v>
       </c>
@@ -14948,7 +14906,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>395</v>
       </c>
@@ -14959,7 +14917,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>200</v>
       </c>
@@ -14967,7 +14925,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>200</v>
       </c>
@@ -14975,7 +14933,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>200</v>
       </c>
@@ -14983,7 +14941,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>200</v>
       </c>
@@ -14991,7 +14949,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>200</v>
       </c>
@@ -14999,7 +14957,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>300</v>
       </c>
@@ -15007,7 +14965,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>300</v>
       </c>
@@ -15015,7 +14973,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>300</v>
       </c>
@@ -15023,7 +14981,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>300</v>
       </c>
@@ -15031,7 +14989,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>300</v>
       </c>
@@ -15039,7 +14997,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>400</v>
       </c>
@@ -15047,7 +15005,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>400</v>
       </c>
@@ -15055,7 +15013,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>400</v>
       </c>
@@ -15063,7 +15021,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>400</v>
       </c>
@@ -15071,7 +15029,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>400</v>
       </c>
@@ -15079,12 +15037,12 @@
         <v>389</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>387</v>
       </c>
@@ -15092,7 +15050,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D24" s="7" t="s">
         <v>385</v>
       </c>
@@ -15100,7 +15058,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D25" s="7" t="s">
         <v>383</v>
       </c>
@@ -15114,7 +15072,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E26" s="7" t="s">
         <v>381</v>
       </c>
@@ -15125,7 +15083,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
         <v>379</v>
       </c>
@@ -15136,7 +15094,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F28" t="s">
         <v>377</v>
       </c>
@@ -15147,7 +15105,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>375</v>
       </c>
@@ -15158,7 +15116,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
         <v>373</v>
       </c>
@@ -15169,7 +15127,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D31" s="7" t="s">
         <v>370</v>
       </c>
@@ -15183,7 +15141,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D32" s="7" t="s">
         <v>367</v>
       </c>
@@ -15197,7 +15155,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D33" s="7" t="s">
         <v>364</v>
       </c>
@@ -15208,7 +15166,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D34" s="22" t="s">
         <v>361</v>
       </c>
@@ -15222,7 +15180,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D35" s="7" t="s">
         <v>359</v>
       </c>
@@ -15236,7 +15194,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D36" s="22" t="s">
         <v>356</v>
       </c>
@@ -15250,7 +15208,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D37" s="7" t="s">
         <v>354</v>
       </c>
@@ -15264,7 +15222,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>350</v>
       </c>
@@ -15272,7 +15230,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
         <v>349</v>
       </c>
@@ -15280,7 +15238,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>347</v>
       </c>
@@ -15291,7 +15249,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
         <v>345</v>
       </c>
@@ -15302,7 +15260,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D42" s="7" t="s">
         <v>342</v>
       </c>
@@ -15310,7 +15268,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
         <v>340</v>
       </c>
@@ -15318,7 +15276,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
         <v>339</v>
       </c>
@@ -15326,7 +15284,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
         <v>337</v>
       </c>
@@ -15334,7 +15292,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D46" s="7" t="s">
         <v>335</v>
       </c>
@@ -15342,7 +15300,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D47" s="7" t="s">
         <v>333</v>
       </c>
@@ -15350,7 +15308,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
         <v>332</v>
       </c>
@@ -15358,7 +15316,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
         <v>330</v>
       </c>
@@ -15366,7 +15324,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D54" t="s">
         <v>329</v>
       </c>
@@ -15380,7 +15338,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D55" t="s">
         <v>322</v>
       </c>
@@ -15394,7 +15352,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D56" t="s">
         <v>320</v>
       </c>
@@ -15405,27 +15363,27 @@
         <v>321</v>
       </c>
     </row>
-    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D57" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="58" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D58" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="60" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="63" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D63" t="s">
         <v>326</v>
       </c>
@@ -15436,7 +15394,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="64" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D64" t="s">
         <v>323</v>
       </c>
@@ -15447,7 +15405,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D65" t="s">
         <v>321</v>
       </c>
@@ -15458,7 +15416,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D66" t="s">
         <v>316</v>
       </c>
@@ -15469,7 +15427,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E67" t="s">
         <v>318</v>
       </c>
@@ -15477,7 +15435,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E68" t="s">
         <v>317</v>
       </c>
@@ -15485,7 +15443,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E69" t="s">
         <v>316</v>
       </c>
@@ -15493,7 +15451,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E70" t="s">
         <v>315</v>
       </c>
@@ -15501,7 +15459,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E71" t="s">
         <v>314</v>
       </c>
@@ -15509,7 +15467,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F72" t="s">
         <v>313</v>
       </c>
@@ -15517,10 +15475,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>